<commit_message>
Local edits before pulling from origin
</commit_message>
<xml_diff>
--- a/IS_2005-07_2008-07.xlsx
+++ b/IS_2005-07_2008-07.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Vol-Adj Trend Analysis</t>
   </si>
@@ -70,22 +70,22 @@
     <t>User Weight</t>
   </si>
   <si>
-    <t>Meridian Strategies</t>
-  </si>
-  <si>
-    <t>Sentinel Global</t>
-  </si>
-  <si>
-    <t>Sentinel Advisors</t>
-  </si>
-  <si>
-    <t>Vista Capital</t>
-  </si>
-  <si>
-    <t>Axiom Holdings</t>
-  </si>
-  <si>
-    <t>Quantum Advisors</t>
+    <t>Forge Advisors</t>
+  </si>
+  <si>
+    <t>Crescent Group</t>
+  </si>
+  <si>
+    <t>Vista Global</t>
+  </si>
+  <si>
+    <t>Forge Group</t>
+  </si>
+  <si>
+    <t>Adaptive Global</t>
+  </si>
+  <si>
+    <t>Adaptive LP</t>
   </si>
   <si>
     <t>EqualWeight_60</t>
@@ -533,34 +533,34 @@
         <v>16</v>
       </c>
       <c r="C6" s="3">
-        <v>3.771265572203131</v>
+        <v>-0.3785348850876669</v>
       </c>
       <c r="D6" s="3">
-        <v>2.85703895554428</v>
+        <v>2.8409709314909</v>
       </c>
       <c r="E6" s="3">
-        <v>1.226945902178641</v>
+        <v>-0.2268126756519981</v>
       </c>
       <c r="F6" s="3">
-        <v>1.806620019236472</v>
+        <v>-0.2130740705930198</v>
       </c>
       <c r="G6" s="4">
-        <v>-2.718127777170887</v>
+        <v>-5.349451854226828</v>
       </c>
       <c r="H6" s="3">
-        <v>2.447961910962637</v>
+        <v>-3.615924393137682</v>
       </c>
       <c r="I6" s="3">
-        <v>1.842519342127739</v>
+        <v>2.528112206147016</v>
       </c>
       <c r="J6" s="3">
-        <v>1.184317867246584</v>
+        <v>-1.535437278864703</v>
       </c>
       <c r="K6" s="3">
-        <v>0.8857021484952906</v>
+        <v>-1.136800703024587</v>
       </c>
       <c r="L6" s="4">
-        <v>-1.194669716913799</v>
+        <v>-3.753007383132034</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -568,34 +568,34 @@
         <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>4.607520676971699</v>
+        <v>-0.3168792914502561</v>
       </c>
       <c r="D7" s="3">
-        <v>2.95218228500657</v>
+        <v>2.942509298682781</v>
       </c>
       <c r="E7" s="3">
-        <v>1.470670481863116</v>
+        <v>-0.1980325516879222</v>
       </c>
       <c r="F7" s="3">
-        <v>1.875702623187282</v>
+        <v>-0.1989919255611703</v>
       </c>
       <c r="G7" s="4">
-        <v>-3.168174268243418</v>
+        <v>-4.721184679050827</v>
       </c>
       <c r="H7" s="3">
-        <v>1.736778935103533</v>
+        <v>-2.583161540300805</v>
       </c>
       <c r="I7" s="3">
-        <v>1.919344040345027</v>
+        <v>2.701070854979653</v>
       </c>
       <c r="J7" s="3">
-        <v>0.7663793310894792</v>
+        <v>-1.054764953085838</v>
       </c>
       <c r="K7" s="3">
-        <v>0.6109521617000697</v>
+        <v>-0.7945078021369302</v>
       </c>
       <c r="L7" s="4">
-        <v>-1.555385973566104</v>
+        <v>-2.756772817697395</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -603,37 +603,37 @@
         <v>18</v>
       </c>
       <c r="B9" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
-        <v>12.3427948654834</v>
+        <v>-2.851214946804337</v>
       </c>
       <c r="D9" s="3">
-        <v>5.455447255899808</v>
+        <v>5.45544725589981</v>
       </c>
       <c r="E9" s="3">
-        <v>2.216391325847431</v>
+        <v>-0.5687166771409815</v>
       </c>
       <c r="F9" s="3">
-        <v>3.02276400639657</v>
+        <v>-0.5200972081214207</v>
       </c>
       <c r="G9" s="4">
-        <v>-4.252113952654735</v>
+        <v>-14.26826671866541</v>
       </c>
       <c r="H9" s="3">
-        <v>-7.286060064230537</v>
+        <v>2.613682116821114</v>
       </c>
       <c r="I9" s="3">
-        <v>3.444528222728684</v>
+        <v>4.022215265623042</v>
       </c>
       <c r="J9" s="3">
-        <v>-2.19243185401495</v>
+        <v>0.5837203203802417</v>
       </c>
       <c r="K9" s="3">
-        <v>-1.458702542533131</v>
+        <v>0.8223133379612338</v>
       </c>
       <c r="L9" s="4">
-        <v>-6.524986051795311</v>
+        <v>-2.373536470462012</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -641,37 +641,37 @@
         <v>19</v>
       </c>
       <c r="B10" s="5">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.8953936574506161</v>
+        <v>3.884049280715574</v>
       </c>
       <c r="D10" s="3">
-        <v>5.455447255899807</v>
+        <v>5.45544725589981</v>
       </c>
       <c r="E10" s="3">
-        <v>-0.2102087129701995</v>
+        <v>0.6658776487845488</v>
       </c>
       <c r="F10" s="3">
-        <v>-0.2214845565172524</v>
+        <v>0.7211994954460942</v>
       </c>
       <c r="G10" s="4">
-        <v>-13.13505190977091</v>
+        <v>-6.629299688635159</v>
       </c>
       <c r="H10" s="3">
-        <v>-1.677394184165693</v>
+        <v>-8.713526365630075</v>
       </c>
       <c r="I10" s="3">
-        <v>5.925084500669564</v>
+        <v>5.387853580090061</v>
       </c>
       <c r="J10" s="3">
-        <v>-0.3279662116682777</v>
+        <v>-1.666593118295786</v>
       </c>
       <c r="K10" s="3">
-        <v>-0.3532386751384517</v>
+        <v>-1.486309745840762</v>
       </c>
       <c r="L10" s="4">
-        <v>-5.32096900656126</v>
+        <v>-8.211035154911572</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -679,37 +679,37 @@
         <v>20</v>
       </c>
       <c r="B11" s="5">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3">
-        <v>-1.325582143002446</v>
+        <v>3.356033138241488</v>
       </c>
       <c r="D11" s="3">
-        <v>5.45544725589981</v>
+        <v>5.455447255899808</v>
       </c>
       <c r="E11" s="3">
-        <v>-0.2890635648957865</v>
+        <v>0.5690906911427056</v>
       </c>
       <c r="F11" s="3">
-        <v>-0.274300806564952</v>
+        <v>0.4843224687471556</v>
       </c>
       <c r="G11" s="4">
-        <v>-7.616875746354324</v>
+        <v>-7.769692220548297</v>
       </c>
       <c r="H11" s="3">
-        <v>8.825704130252831</v>
+        <v>-1.327377915638495</v>
       </c>
       <c r="I11" s="3">
-        <v>5.7733059195707</v>
+        <v>4.708869920302339</v>
       </c>
       <c r="J11" s="3">
-        <v>1.482663644741695</v>
+        <v>-0.3383425908842123</v>
       </c>
       <c r="K11" s="3">
-        <v>2.768262178174099</v>
+        <v>-0.3324762823701682</v>
       </c>
       <c r="L11" s="4">
-        <v>-2.391322032338505</v>
+        <v>-4.039572413768411</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -717,37 +717,37 @@
         <v>21</v>
       </c>
       <c r="B12" s="5">
-        <v>29</v>
+        <v>7.000000000000001</v>
       </c>
       <c r="C12" s="3">
-        <v>8.624558393084204</v>
+        <v>-1.340449526914833</v>
       </c>
       <c r="D12" s="3">
         <v>5.45544725589981</v>
       </c>
       <c r="E12" s="3">
-        <v>1.534827322386836</v>
+        <v>-0.2917888013823658</v>
       </c>
       <c r="F12" s="3">
-        <v>1.676952332716793</v>
+        <v>-0.2582406241972316</v>
       </c>
       <c r="G12" s="4">
-        <v>-4.403278743302941</v>
+        <v>-9.756021348966915</v>
       </c>
       <c r="H12" s="3">
-        <v>-1.974309814725583</v>
+        <v>-7.140595322606947</v>
       </c>
       <c r="I12" s="3">
-        <v>6.276784652174086</v>
+        <v>4.132552664456281</v>
       </c>
       <c r="J12" s="3">
-        <v>-0.3568934211058204</v>
+        <v>-1.792216399234864</v>
       </c>
       <c r="K12" s="3">
-        <v>-0.192981836204243</v>
+        <v>-1.516744995537287</v>
       </c>
       <c r="L12" s="4">
-        <v>-8.211992932318813</v>
+        <v>-8.204845222930768</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -755,37 +755,37 @@
         <v>22</v>
       </c>
       <c r="B13" s="5">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3">
-        <v>2.750816417701518</v>
+        <v>-2.350745983204072</v>
       </c>
       <c r="D13" s="3">
         <v>5.45544725589981</v>
       </c>
       <c r="E13" s="3">
-        <v>0.4581526337936117</v>
+        <v>-0.4769792007940091</v>
       </c>
       <c r="F13" s="3">
-        <v>0.5224165853963869</v>
+        <v>-0.4455235076622012</v>
       </c>
       <c r="G13" s="4">
-        <v>-5.010994841559702</v>
+        <v>-13.14186754769434</v>
       </c>
       <c r="H13" s="3">
-        <v>3.855795457756028</v>
+        <v>3.391684246988902</v>
       </c>
       <c r="I13" s="3">
-        <v>6.341625464845499</v>
+        <v>4.712233996886236</v>
       </c>
       <c r="J13" s="3">
-        <v>0.5660949458973067</v>
+        <v>0.6633479822354064</v>
       </c>
       <c r="K13" s="3">
-        <v>0.4704505562580215</v>
+        <v>0.960662793023961</v>
       </c>
       <c r="L13" s="4">
-        <v>-4.244086245079648</v>
+        <v>-2.769445044287977</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -793,37 +793,37 @@
         <v>23</v>
       </c>
       <c r="B14" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3">
-        <v>1.124111705374742</v>
+        <v>-3.381520856782139</v>
       </c>
       <c r="D14" s="3">
-        <v>5.455447255899812</v>
+        <v>5.45544725589981</v>
       </c>
       <c r="E14" s="3">
-        <v>0.159972734690459</v>
+        <v>-0.6659233560992102</v>
       </c>
       <c r="F14" s="3">
-        <v>0.1568119198868004</v>
+        <v>-0.5573742325437002</v>
       </c>
       <c r="G14" s="4">
-        <v>-9.327602305081884</v>
+        <v>-12.74098237107393</v>
       </c>
       <c r="H14" s="3">
-        <v>13.33253767466478</v>
+        <v>-10.28222507670823</v>
       </c>
       <c r="I14" s="3">
-        <v>6.211044251361618</v>
+        <v>7.398203870187875</v>
       </c>
       <c r="J14" s="3">
-        <v>2.10378542037708</v>
+        <v>-1.425759359315101</v>
       </c>
       <c r="K14" s="3">
-        <v>3.162634574236533</v>
+        <v>-1.059064871216358</v>
       </c>
       <c r="L14" s="4">
-        <v>-1.896768227337409</v>
+        <v>-10.59027475909533</v>
       </c>
     </row>
     <row r="16" spans="1:13">

</xml_diff>